<commit_message>
Updated script with new sources
</commit_message>
<xml_diff>
--- a/Jeff_Wilson_Sources.xlsx
+++ b/Jeff_Wilson_Sources.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,6 +552,91 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Jeff Wilson (Instagram)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/profdumpster/?hl=am-et</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Instagram profile.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Jeff Wilson (YouTube Interview)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=bhuUdCseF3k</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>YouTube interview with Jeff Wilson.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Jeff Wilson (Initialized Blog)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://blog.initialized.com/2022/10/video-interview-with-jeff-wilson-ceo-of-jupe/</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Blog interview with Jeff Wilson, CEO of Jupe.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Jeff Wilson (Miami Ad School)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://miamiadschool.com/event/jeff-wilson-jupe/</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Event at Miami Ad School featuring Jeff Wilson.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Jeff Wilson (Capital Letter)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://www.capitalletter.com/p/jupe</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Article on Jupe in Capital Letter.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>